<commit_message>
FIX: Corrected stoichiometic factor in Streeter-Phelps example
</commit_message>
<xml_diff>
--- a/inst/examples/streeterPhelpsLike/def_tables.xlsx
+++ b/inst/examples/streeterPhelpsLike/def_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="297" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="157" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -347,7 +347,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -553,7 +553,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -589,8 +589,8 @@
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>